<commit_message>
add more advanced versions of tests
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D8FD2796-5EDC-4966-806F-9C8BECCA9FC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E410A36B-4CA5-494F-AAF6-8CC115326F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="18000" windowHeight="9375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="18030" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meal Search Results" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add final version of Project
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E410A36B-4CA5-494F-AAF6-8CC115326F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPRIKQ\Dragan\The Final Project QA\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9BE305-DE0D-48F0-8E9D-33DF71DB4306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="18030" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Meal Search Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Meal Search Results" sheetId="3" r:id="rId1"/>
     <sheet name="Meals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -195,13 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -419,26 +422,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:X22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9CDE44-F6A6-43E8-BFAD-6814A38566A5}">
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8:XFD61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="59" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,215 +442,170 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="R7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="S7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="T7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="U7" s="3" t="s">
+      <c r="U7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="3" t="s">
+      <c r="V7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="W7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="X7" s="3" t="s">
+      <c r="X7" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A1E5A927-CE9F-49A9-98DB-21F3C77E4954}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{EA98D804-F028-4D17-A337-D4B24E89AD3D}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{AB3A94CF-CFA0-4C66-AFF8-5BE439CEC2F0}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{CFF9447A-5AA8-4C5B-9523-463940B62295}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{C2F65DCD-C958-46C3-B309-3BF2DD98944E}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{99F29D5B-EC4A-4181-9601-86023AA8986D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -683,27 +631,27 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>